<commit_message>
Made changes to Testutil.java
</commit_message>
<xml_diff>
--- a/Xls/src/data/TestCases.xlsx
+++ b/Xls/src/data/TestCases.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="11115" windowHeight="2385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="11115" windowHeight="2385" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
     <sheet name="Test Steps" sheetId="3" r:id="rId2"/>
     <sheet name="Data" sheetId="1" r:id="rId3"/>
+    <sheet name="DataTest" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:H6"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="60">
   <si>
     <t>LoginTest</t>
   </si>
@@ -140,6 +140,63 @@
   </si>
   <si>
     <t>prodTab</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>MM1</t>
+  </si>
+  <si>
+    <t>MM2</t>
+  </si>
+  <si>
+    <t>MM3</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>DataO</t>
+  </si>
+  <si>
+    <t>DataT</t>
+  </si>
+  <si>
+    <t>DataF</t>
   </si>
 </sst>
 </file>
@@ -567,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -760,7 +817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -956,4 +1013,92 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>